<commit_message>
alignment tree and aligners. various corrections.
</commit_message>
<xml_diff>
--- a/tabular/3. BTV DB all segs 2016-06-22_data_missing.xlsx
+++ b/tabular/3. BTV DB all segs 2016-06-22_data_missing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="7380" windowWidth="24900" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="16660" yWindow="8340" windowWidth="24900" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="query_result.csv" sheetId="1" r:id="rId1"/>
@@ -14907,8 +14907,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1617">
+  <cellStyleXfs count="1619">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -16557,7 +16559,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1617">
+  <cellStyles count="1619">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -17366,6 +17368,7 @@
     <cellStyle name="Followed Hyperlink" xfId="1612" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1614" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1616" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1618" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -18174,6 +18177,7 @@
     <cellStyle name="Hyperlink" xfId="1611" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1613" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1615" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1617" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -18505,9 +18509,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4470"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4403" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I4418" sqref="A1:K4470"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1022" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1037" sqref="D1037"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -36401,7 +36405,7 @@
         <v>1109</v>
       </c>
       <c r="D1033" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G1033" s="2" t="s">
         <v>602</v>
@@ -36418,7 +36422,7 @@
         <v>1110</v>
       </c>
       <c r="D1034" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G1034" s="2" t="s">
         <v>602</v>
@@ -36435,7 +36439,7 @@
         <v>1111</v>
       </c>
       <c r="D1035" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G1035" s="2" t="s">
         <v>602</v>
@@ -42549,7 +42553,7 @@
         <v>1510</v>
       </c>
       <c r="D1419" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1420" spans="1:4">
@@ -42563,7 +42567,7 @@
         <v>1511</v>
       </c>
       <c r="D1420" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1421" spans="1:4">
@@ -42591,7 +42595,7 @@
         <v>1513</v>
       </c>
       <c r="D1422" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1423" spans="1:4">
@@ -42605,7 +42609,7 @@
         <v>1514</v>
       </c>
       <c r="D1423" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1424" spans="1:4">
@@ -42619,7 +42623,7 @@
         <v>1515</v>
       </c>
       <c r="D1424" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="1425" spans="1:9">

</xml_diff>

<commit_message>
additional missing country data from kiki
</commit_message>
<xml_diff>
--- a/tabular/3. BTV DB all segs 2016-06-22_data_missing.xlsx
+++ b/tabular/3. BTV DB all segs 2016-06-22_data_missing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="16660" yWindow="8340" windowWidth="24900" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="3620" yWindow="8520" windowWidth="42500" windowHeight="15780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="query_result.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16820" uniqueCount="4943">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16941" uniqueCount="4947">
   <si>
     <t>sequence_id</t>
   </si>
@@ -14848,6 +14848,18 @@
   </si>
   <si>
     <t>gb_segment_missing</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>West Java - Indonesia</t>
   </si>
 </sst>
 </file>
@@ -14907,8 +14919,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1619">
+  <cellStyleXfs count="1629">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -16559,7 +16581,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1619">
+  <cellStyles count="1629">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -17369,6 +17391,11 @@
     <cellStyle name="Followed Hyperlink" xfId="1614" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1616" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1618" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1620" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1622" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1624" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1626" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1628" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -18178,6 +18205,11 @@
     <cellStyle name="Hyperlink" xfId="1613" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1615" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1617" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1619" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1621" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1623" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1625" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1627" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -18510,8 +18542,8 @@
   <dimension ref="A1:M4470"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1022" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1037" sqref="D1037"/>
+      <pane ySplit="1" topLeftCell="A4445" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G4464" sqref="G4464"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -27283,6 +27315,9 @@
       <c r="D576" s="2">
         <v>2</v>
       </c>
+      <c r="G576" s="2" t="s">
+        <v>616</v>
+      </c>
       <c r="K576" s="2">
         <v>23</v>
       </c>
@@ -27303,6 +27338,9 @@
       <c r="F577" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G577" s="2" t="s">
+        <v>4943</v>
+      </c>
     </row>
     <row r="578" spans="1:11">
       <c r="A578" s="2" t="s">
@@ -27320,6 +27358,9 @@
       <c r="F578" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G578" s="2" t="s">
+        <v>4943</v>
+      </c>
     </row>
     <row r="579" spans="1:11">
       <c r="A579" s="2" t="s">
@@ -27337,6 +27378,9 @@
       <c r="F579" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="G579" s="2" t="s">
+        <v>4943</v>
+      </c>
     </row>
     <row r="580" spans="1:11">
       <c r="A580" s="2" t="s">
@@ -28531,6 +28575,9 @@
       <c r="E651" s="7" t="s">
         <v>4756</v>
       </c>
+      <c r="G651" s="4" t="s">
+        <v>699</v>
+      </c>
       <c r="H651" s="4">
         <v>1962</v>
       </c>
@@ -28552,6 +28599,9 @@
       <c r="E652" s="7" t="s">
         <v>4757</v>
       </c>
+      <c r="G652" s="4" t="s">
+        <v>699</v>
+      </c>
       <c r="H652" s="4">
         <v>1976</v>
       </c>
@@ -28573,6 +28623,9 @@
       <c r="E653" s="7" t="s">
         <v>4756</v>
       </c>
+      <c r="G653" s="4" t="s">
+        <v>699</v>
+      </c>
       <c r="H653" s="4">
         <v>1976</v>
       </c>
@@ -28594,6 +28647,9 @@
       <c r="E654" s="7" t="s">
         <v>4757</v>
       </c>
+      <c r="G654" s="4" t="s">
+        <v>699</v>
+      </c>
       <c r="H654" s="4">
         <v>1962</v>
       </c>
@@ -30628,6 +30684,9 @@
       <c r="E746" s="1" t="s">
         <v>4787</v>
       </c>
+      <c r="G746" s="2" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="747" spans="1:11">
       <c r="A747" s="2" t="s">
@@ -30642,6 +30701,9 @@
       <c r="E747" s="1" t="s">
         <v>4788</v>
       </c>
+      <c r="G747" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="748" spans="1:11">
       <c r="A748" s="2" t="s">
@@ -30656,6 +30718,9 @@
       <c r="E748" s="1" t="s">
         <v>4789</v>
       </c>
+      <c r="G748" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K748" s="2">
         <v>2</v>
       </c>
@@ -30673,6 +30738,9 @@
       <c r="E749" s="1" t="s">
         <v>767</v>
       </c>
+      <c r="G749" s="2" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="750" spans="1:11">
       <c r="A750" s="2" t="s">
@@ -30687,6 +30755,9 @@
       <c r="E750" s="1" t="s">
         <v>4790</v>
       </c>
+      <c r="G750" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K750" s="2">
         <v>2</v>
       </c>
@@ -30704,6 +30775,9 @@
       <c r="E751" s="1" t="s">
         <v>4791</v>
       </c>
+      <c r="G751" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K751" s="2">
         <v>4</v>
       </c>
@@ -35071,6 +35145,9 @@
       <c r="F968" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="G968" s="2" t="s">
+        <v>4944</v>
+      </c>
       <c r="H968" s="2">
         <v>2001</v>
       </c>
@@ -35239,6 +35316,9 @@
       <c r="F974" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="G974" s="2" t="s">
+        <v>4944</v>
+      </c>
       <c r="H974" s="2">
         <v>2001</v>
       </c>
@@ -35420,6 +35500,9 @@
       <c r="C982" s="2" t="s">
         <v>1057</v>
       </c>
+      <c r="G982" s="2" t="s">
+        <v>4945</v>
+      </c>
       <c r="H982" s="2">
         <v>1999</v>
       </c>
@@ -35852,6 +35935,9 @@
       <c r="F1003" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="G1003" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="H1003" s="2">
         <v>1990</v>
       </c>
@@ -35872,6 +35958,9 @@
       <c r="F1004" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="G1004" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K1004" s="2">
         <v>10</v>
       </c>
@@ -36179,6 +36268,9 @@
       <c r="F1021" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G1021" s="2" t="s">
+        <v>4946</v>
+      </c>
     </row>
     <row r="1022" spans="1:11">
       <c r="A1022" s="2" t="s">
@@ -37245,6 +37337,9 @@
       <c r="E1077" s="1" t="s">
         <v>4807</v>
       </c>
+      <c r="G1077" s="2" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="1078" spans="1:9">
       <c r="A1078" s="2" t="s">
@@ -37262,6 +37357,9 @@
       <c r="E1078" s="1" t="s">
         <v>4808</v>
       </c>
+      <c r="G1078" s="2" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="1079" spans="1:9">
       <c r="A1079" s="2" t="s">
@@ -37279,6 +37377,9 @@
       <c r="E1079" s="1" t="s">
         <v>4809</v>
       </c>
+      <c r="G1079" s="2" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="1080" spans="1:9">
       <c r="A1080" s="2" t="s">
@@ -37296,6 +37397,9 @@
       <c r="E1080" s="1" t="s">
         <v>4810</v>
       </c>
+      <c r="G1080" s="2" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="1081" spans="1:9">
       <c r="A1081" s="2" t="s">
@@ -37313,6 +37417,9 @@
       <c r="E1081" s="1" t="s">
         <v>4811</v>
       </c>
+      <c r="G1081" s="2" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="1082" spans="1:9">
       <c r="A1082" s="2" t="s">
@@ -37330,6 +37437,9 @@
       <c r="E1082" s="1" t="s">
         <v>4812</v>
       </c>
+      <c r="G1082" s="2" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="1083" spans="1:9">
       <c r="A1083" s="2" t="s">
@@ -37347,6 +37457,9 @@
       <c r="E1083" s="1" t="s">
         <v>4813</v>
       </c>
+      <c r="G1083" s="2" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="1084" spans="1:9">
       <c r="A1084" s="2" t="s">
@@ -37364,6 +37477,9 @@
       <c r="E1084" s="1" t="s">
         <v>4814</v>
       </c>
+      <c r="G1084" s="2" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="1085" spans="1:9">
       <c r="A1085" s="2" t="s">
@@ -38710,6 +38826,9 @@
       <c r="D1169" s="2">
         <v>2</v>
       </c>
+      <c r="G1169" s="2" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="1170" spans="1:8">
       <c r="A1170" s="2" t="s">
@@ -38735,6 +38854,9 @@
       <c r="C1171" s="2" t="s">
         <v>1252</v>
       </c>
+      <c r="G1171" s="2" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="1172" spans="1:8">
       <c r="A1172" s="2" t="s">
@@ -38746,6 +38868,9 @@
       <c r="C1172" s="2" t="s">
         <v>1254</v>
       </c>
+      <c r="G1172" s="2" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="1173" spans="1:8">
       <c r="A1173" s="2" t="s">
@@ -38757,6 +38882,9 @@
       <c r="C1173" s="2" t="s">
         <v>1256</v>
       </c>
+      <c r="G1173" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="1174" spans="1:8">
       <c r="A1174" s="2" t="s">
@@ -38768,6 +38896,9 @@
       <c r="C1174" s="2" t="s">
         <v>1258</v>
       </c>
+      <c r="G1174" s="2" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="1175" spans="1:8">
       <c r="A1175" s="2" t="s">
@@ -38895,6 +39026,9 @@
       <c r="D1182" s="2">
         <v>6</v>
       </c>
+      <c r="G1182" s="2" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="1183" spans="1:8">
       <c r="A1183" s="2" t="s">
@@ -38909,6 +39043,9 @@
       <c r="D1183" s="2">
         <v>6</v>
       </c>
+      <c r="G1183" s="2" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="1184" spans="1:8">
       <c r="A1184" s="2" t="s">
@@ -38923,6 +39060,9 @@
       <c r="D1184" s="2">
         <v>6</v>
       </c>
+      <c r="G1184" s="2" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="1185" spans="1:8">
       <c r="A1185" s="2" t="s">
@@ -38937,6 +39077,9 @@
       <c r="D1185" s="2">
         <v>6</v>
       </c>
+      <c r="G1185" s="2" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="1186" spans="1:8">
       <c r="A1186" s="2" t="s">
@@ -38951,6 +39094,9 @@
       <c r="D1186" s="2">
         <v>6</v>
       </c>
+      <c r="G1186" s="2" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="1187" spans="1:8">
       <c r="A1187" s="2" t="s">
@@ -38965,6 +39111,9 @@
       <c r="D1187" s="2">
         <v>6</v>
       </c>
+      <c r="G1187" s="2" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="1188" spans="1:8">
       <c r="A1188" s="2" t="s">
@@ -42084,6 +42233,9 @@
       <c r="C1386" s="2" t="s">
         <v>1477</v>
       </c>
+      <c r="G1386" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="K1386" s="2">
         <v>4</v>
       </c>
@@ -43444,6 +43596,9 @@
       <c r="E1472" s="1" t="s">
         <v>4830</v>
       </c>
+      <c r="G1472" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="1473" spans="1:9">
       <c r="A1473" s="2" t="s">
@@ -43461,6 +43616,9 @@
       <c r="E1473" s="1" t="s">
         <v>4831</v>
       </c>
+      <c r="G1473" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="1474" spans="1:9">
       <c r="A1474" s="2" t="s">
@@ -43478,6 +43636,9 @@
       <c r="E1474" s="1" t="s">
         <v>4832</v>
       </c>
+      <c r="G1474" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="1475" spans="1:9">
       <c r="A1475" s="2" t="s">
@@ -43495,6 +43656,9 @@
       <c r="E1475" s="1" t="s">
         <v>4833</v>
       </c>
+      <c r="G1475" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="1476" spans="1:9">
       <c r="A1476" s="2" t="s">
@@ -43512,6 +43676,9 @@
       <c r="E1476" s="1" t="s">
         <v>4834</v>
       </c>
+      <c r="G1476" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="1477" spans="1:9">
       <c r="A1477" s="2" t="s">
@@ -43529,6 +43696,9 @@
       <c r="E1477" s="1" t="s">
         <v>4835</v>
       </c>
+      <c r="G1477" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="1478" spans="1:9">
       <c r="A1478" s="2" t="s">
@@ -43546,6 +43716,9 @@
       <c r="E1478" s="1" t="s">
         <v>4836</v>
       </c>
+      <c r="G1478" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="1479" spans="1:9">
       <c r="A1479" s="2" t="s">
@@ -43563,6 +43736,9 @@
       <c r="E1479" s="1" t="s">
         <v>4837</v>
       </c>
+      <c r="G1479" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="1480" spans="1:9">
       <c r="A1480" s="2" t="s">
@@ -43580,6 +43756,9 @@
       <c r="E1480" s="1" t="s">
         <v>4838</v>
       </c>
+      <c r="G1480" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="1481" spans="1:9">
       <c r="A1481" s="2" t="s">
@@ -43597,6 +43776,9 @@
       <c r="E1481" s="1" t="s">
         <v>4839</v>
       </c>
+      <c r="G1481" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="1482" spans="1:9">
       <c r="A1482" s="2" t="s">
@@ -43614,6 +43796,9 @@
       <c r="E1482" s="1" t="s">
         <v>4840</v>
       </c>
+      <c r="G1482" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="1483" spans="1:9">
       <c r="A1483" s="2" t="s">
@@ -43631,6 +43816,9 @@
       <c r="E1483" s="1" t="s">
         <v>4841</v>
       </c>
+      <c r="G1483" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="1484" spans="1:9">
       <c r="A1484" s="2" t="s">
@@ -43648,6 +43836,9 @@
       <c r="E1484" s="1" t="s">
         <v>4842</v>
       </c>
+      <c r="G1484" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="1485" spans="1:9">
       <c r="A1485" s="2" t="s">
@@ -43665,6 +43856,9 @@
       <c r="E1485" s="1" t="s">
         <v>4843</v>
       </c>
+      <c r="G1485" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="1486" spans="1:9">
       <c r="A1486" s="2" t="s">
@@ -43682,6 +43876,9 @@
       <c r="E1486" s="1" t="s">
         <v>4844</v>
       </c>
+      <c r="G1486" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="1487" spans="1:9">
       <c r="A1487" s="2" t="s">
@@ -43699,6 +43896,9 @@
       <c r="E1487" s="1" t="s">
         <v>4845</v>
       </c>
+      <c r="G1487" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="1488" spans="1:9">
       <c r="A1488" s="2" t="s">
@@ -54165,6 +54365,9 @@
       <c r="E2146" s="1" t="s">
         <v>4876</v>
       </c>
+      <c r="G2146" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2147" spans="1:9">
       <c r="A2147" s="2" t="s">
@@ -54179,6 +54382,9 @@
       <c r="E2147" s="1" t="s">
         <v>4876</v>
       </c>
+      <c r="G2147" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2148" spans="1:9">
       <c r="A2148" s="2" t="s">
@@ -54193,6 +54399,9 @@
       <c r="E2148" s="1" t="s">
         <v>4876</v>
       </c>
+      <c r="G2148" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2149" spans="1:9">
       <c r="A2149" s="2" t="s">
@@ -54207,6 +54416,9 @@
       <c r="E2149" s="1" t="s">
         <v>4876</v>
       </c>
+      <c r="G2149" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2150" spans="1:9">
       <c r="A2150" s="2" t="s">
@@ -54221,6 +54433,9 @@
       <c r="E2150" s="1" t="s">
         <v>4876</v>
       </c>
+      <c r="G2150" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2151" spans="1:9">
       <c r="A2151" s="2" t="s">
@@ -54235,6 +54450,9 @@
       <c r="E2151" s="1" t="s">
         <v>4876</v>
       </c>
+      <c r="G2151" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2152" spans="1:9">
       <c r="A2152" s="2" t="s">
@@ -54249,6 +54467,9 @@
       <c r="E2152" s="1" t="s">
         <v>4876</v>
       </c>
+      <c r="G2152" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2153" spans="1:9">
       <c r="A2153" s="2" t="s">
@@ -54263,6 +54484,9 @@
       <c r="E2153" s="1" t="s">
         <v>4876</v>
       </c>
+      <c r="G2153" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2154" spans="1:9">
       <c r="A2154" s="2" t="s">
@@ -54277,6 +54501,9 @@
       <c r="E2154" s="1" t="s">
         <v>4876</v>
       </c>
+      <c r="G2154" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2155" spans="1:9">
       <c r="A2155" s="2" t="s">
@@ -54291,6 +54518,9 @@
       <c r="E2155" s="1" t="s">
         <v>4876</v>
       </c>
+      <c r="G2155" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2156" spans="1:9">
       <c r="A2156" s="2" t="s">
@@ -54305,6 +54535,9 @@
       <c r="E2156" s="1" t="s">
         <v>4877</v>
       </c>
+      <c r="G2156" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2157" spans="1:9">
       <c r="A2157" s="2" t="s">
@@ -54319,6 +54552,9 @@
       <c r="E2157" s="1" t="s">
         <v>4877</v>
       </c>
+      <c r="G2157" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2158" spans="1:9">
       <c r="A2158" s="2" t="s">
@@ -54333,6 +54569,9 @@
       <c r="E2158" s="1" t="s">
         <v>4877</v>
       </c>
+      <c r="G2158" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2159" spans="1:9">
       <c r="A2159" s="2" t="s">
@@ -54347,6 +54586,9 @@
       <c r="E2159" s="1" t="s">
         <v>4877</v>
       </c>
+      <c r="G2159" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2160" spans="1:9">
       <c r="A2160" s="2" t="s">
@@ -54361,8 +54603,11 @@
       <c r="E2160" s="1" t="s">
         <v>4877</v>
       </c>
-    </row>
-    <row r="2161" spans="1:5">
+      <c r="G2160" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2161" spans="1:7">
       <c r="A2161" s="2" t="s">
         <v>2265</v>
       </c>
@@ -54375,8 +54620,11 @@
       <c r="E2161" s="1" t="s">
         <v>4877</v>
       </c>
-    </row>
-    <row r="2162" spans="1:5">
+      <c r="G2161" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2162" spans="1:7">
       <c r="A2162" s="2" t="s">
         <v>2266</v>
       </c>
@@ -54389,8 +54637,11 @@
       <c r="E2162" s="1" t="s">
         <v>4877</v>
       </c>
-    </row>
-    <row r="2163" spans="1:5">
+      <c r="G2162" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2163" spans="1:7">
       <c r="A2163" s="2" t="s">
         <v>2267</v>
       </c>
@@ -54403,8 +54654,11 @@
       <c r="E2163" s="1" t="s">
         <v>4877</v>
       </c>
-    </row>
-    <row r="2164" spans="1:5">
+      <c r="G2163" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2164" spans="1:7">
       <c r="A2164" s="2" t="s">
         <v>2268</v>
       </c>
@@ -54417,8 +54671,11 @@
       <c r="E2164" s="1" t="s">
         <v>4877</v>
       </c>
-    </row>
-    <row r="2165" spans="1:5">
+      <c r="G2164" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2165" spans="1:7">
       <c r="A2165" s="2" t="s">
         <v>2269</v>
       </c>
@@ -54431,8 +54688,11 @@
       <c r="E2165" s="1" t="s">
         <v>4877</v>
       </c>
-    </row>
-    <row r="2166" spans="1:5">
+      <c r="G2165" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2166" spans="1:7">
       <c r="A2166" s="2" t="s">
         <v>2270</v>
       </c>
@@ -54446,7 +54706,7 @@
         <v>4878</v>
       </c>
     </row>
-    <row r="2167" spans="1:5">
+    <row r="2167" spans="1:7">
       <c r="A2167" s="2" t="s">
         <v>2271</v>
       </c>
@@ -54460,7 +54720,7 @@
         <v>4878</v>
       </c>
     </row>
-    <row r="2168" spans="1:5">
+    <row r="2168" spans="1:7">
       <c r="A2168" s="2" t="s">
         <v>2272</v>
       </c>
@@ -54474,7 +54734,7 @@
         <v>4878</v>
       </c>
     </row>
-    <row r="2169" spans="1:5">
+    <row r="2169" spans="1:7">
       <c r="A2169" s="2" t="s">
         <v>2273</v>
       </c>
@@ -54488,7 +54748,7 @@
         <v>4878</v>
       </c>
     </row>
-    <row r="2170" spans="1:5">
+    <row r="2170" spans="1:7">
       <c r="A2170" s="2" t="s">
         <v>2274</v>
       </c>
@@ -54502,7 +54762,7 @@
         <v>4878</v>
       </c>
     </row>
-    <row r="2171" spans="1:5">
+    <row r="2171" spans="1:7">
       <c r="A2171" s="2" t="s">
         <v>2275</v>
       </c>
@@ -54516,7 +54776,7 @@
         <v>4878</v>
       </c>
     </row>
-    <row r="2172" spans="1:5">
+    <row r="2172" spans="1:7">
       <c r="A2172" s="2" t="s">
         <v>2276</v>
       </c>
@@ -54530,7 +54790,7 @@
         <v>4878</v>
       </c>
     </row>
-    <row r="2173" spans="1:5">
+    <row r="2173" spans="1:7">
       <c r="A2173" s="2" t="s">
         <v>2277</v>
       </c>
@@ -54544,7 +54804,7 @@
         <v>4878</v>
       </c>
     </row>
-    <row r="2174" spans="1:5">
+    <row r="2174" spans="1:7">
       <c r="A2174" s="2" t="s">
         <v>2278</v>
       </c>
@@ -54558,7 +54818,7 @@
         <v>4878</v>
       </c>
     </row>
-    <row r="2175" spans="1:5">
+    <row r="2175" spans="1:7">
       <c r="A2175" s="2" t="s">
         <v>2279</v>
       </c>
@@ -54572,7 +54832,7 @@
         <v>4878</v>
       </c>
     </row>
-    <row r="2176" spans="1:5">
+    <row r="2176" spans="1:7">
       <c r="A2176" s="2" t="s">
         <v>2280</v>
       </c>
@@ -60507,6 +60767,9 @@
       <c r="C2592" s="2" t="s">
         <v>2697</v>
       </c>
+      <c r="G2592" s="2" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="2593" spans="1:9">
       <c r="A2593" s="2" t="s">
@@ -64224,6 +64487,9 @@
       <c r="C2874" s="2" t="s">
         <v>2980</v>
       </c>
+      <c r="G2874" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="K2874" s="2">
         <v>11</v>
       </c>
@@ -64238,6 +64504,9 @@
       <c r="C2875" s="2" t="s">
         <v>2981</v>
       </c>
+      <c r="G2875" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="K2875" s="2">
         <v>7</v>
       </c>
@@ -64252,6 +64521,9 @@
       <c r="C2876" s="2" t="s">
         <v>2982</v>
       </c>
+      <c r="G2876" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="K2876" s="2">
         <v>2</v>
       </c>
@@ -64266,6 +64538,9 @@
       <c r="C2877" s="2" t="s">
         <v>2983</v>
       </c>
+      <c r="G2877" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="K2877" s="2">
         <v>16</v>
       </c>
@@ -64280,6 +64555,9 @@
       <c r="C2878" s="2" t="s">
         <v>2984</v>
       </c>
+      <c r="G2878" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="K2878" s="2">
         <v>22</v>
       </c>
@@ -64294,6 +64572,9 @@
       <c r="C2879" s="2" t="s">
         <v>2985</v>
       </c>
+      <c r="G2879" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="K2879" s="2">
         <v>19</v>
       </c>
@@ -64308,6 +64589,9 @@
       <c r="C2880" s="2" t="s">
         <v>2986</v>
       </c>
+      <c r="G2880" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="K2880" s="2">
         <v>23</v>
       </c>
@@ -64322,6 +64606,9 @@
       <c r="C2881" s="2" t="s">
         <v>2987</v>
       </c>
+      <c r="G2881" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="K2881" s="2">
         <v>21</v>
       </c>
@@ -64336,6 +64623,9 @@
       <c r="C2882" s="2" t="s">
         <v>2988</v>
       </c>
+      <c r="G2882" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="K2882" s="2">
         <v>20</v>
       </c>
@@ -64350,6 +64640,9 @@
       <c r="C2883" s="2" t="s">
         <v>2989</v>
       </c>
+      <c r="G2883" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="K2883" s="2">
         <v>8</v>
       </c>
@@ -64364,6 +64657,9 @@
       <c r="C2884" s="2" t="s">
         <v>2990</v>
       </c>
+      <c r="G2884" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2885" spans="1:11">
       <c r="A2885" s="2" t="s">
@@ -85043,6 +85339,9 @@
       <c r="D4325" s="2">
         <v>10</v>
       </c>
+      <c r="G4325" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4325" s="2">
         <v>2</v>
       </c>
@@ -85060,6 +85359,9 @@
       <c r="D4326" s="2">
         <v>10</v>
       </c>
+      <c r="G4326" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4326" s="2">
         <v>13</v>
       </c>
@@ -85077,6 +85379,9 @@
       <c r="D4327" s="2">
         <v>10</v>
       </c>
+      <c r="G4327" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4327" s="2">
         <v>17</v>
       </c>
@@ -85094,6 +85399,9 @@
       <c r="D4328" s="2">
         <v>10</v>
       </c>
+      <c r="G4328" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4328" s="2">
         <v>11</v>
       </c>
@@ -85114,6 +85422,9 @@
       <c r="E4329" s="1" t="s">
         <v>4898</v>
       </c>
+      <c r="G4329" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4329" s="2">
         <v>2</v>
       </c>
@@ -85134,6 +85445,9 @@
       <c r="E4330" s="1" t="s">
         <v>4899</v>
       </c>
+      <c r="G4330" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4330" s="2">
         <v>11</v>
       </c>
@@ -85154,6 +85468,9 @@
       <c r="E4331" s="1" t="s">
         <v>4900</v>
       </c>
+      <c r="G4331" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4331" s="2">
         <v>17</v>
       </c>
@@ -85174,6 +85491,9 @@
       <c r="E4332" s="1" t="s">
         <v>4901</v>
       </c>
+      <c r="G4332" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4332" s="2">
         <v>13</v>
       </c>
@@ -85374,6 +85694,9 @@
       <c r="F4342" s="2" t="s">
         <v>4468</v>
       </c>
+      <c r="G4342" s="2" t="s">
+        <v>616</v>
+      </c>
       <c r="K4342" s="2">
         <v>15</v>
       </c>
@@ -85417,6 +85740,9 @@
       <c r="D4344" s="2">
         <v>2</v>
       </c>
+      <c r="G4344" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4344" s="2">
         <v>13</v>
       </c>
@@ -85434,6 +85760,9 @@
       <c r="D4345" s="2">
         <v>2</v>
       </c>
+      <c r="G4345" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4345" s="2">
         <v>13</v>
       </c>
@@ -85451,6 +85780,9 @@
       <c r="D4346" s="2">
         <v>4</v>
       </c>
+      <c r="G4346" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4346" s="2">
         <v>10</v>
       </c>
@@ -85468,6 +85800,9 @@
       <c r="D4347" s="2">
         <v>6</v>
       </c>
+      <c r="G4347" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4347" s="2">
         <v>11</v>
       </c>
@@ -85485,6 +85820,9 @@
       <c r="D4348" s="2">
         <v>3</v>
       </c>
+      <c r="G4348" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4348" s="2">
         <v>2</v>
       </c>
@@ -85502,6 +85840,9 @@
       <c r="D4349" s="2">
         <v>3</v>
       </c>
+      <c r="G4349" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4349" s="2">
         <v>11</v>
       </c>
@@ -85519,6 +85860,9 @@
       <c r="D4350" s="2">
         <v>3</v>
       </c>
+      <c r="G4350" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4350" s="2">
         <v>13</v>
       </c>
@@ -85536,6 +85880,9 @@
       <c r="D4351" s="2">
         <v>1</v>
       </c>
+      <c r="G4351" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4351" s="2">
         <v>11</v>
       </c>
@@ -85553,6 +85900,9 @@
       <c r="D4352" s="2">
         <v>1</v>
       </c>
+      <c r="G4352" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4352" s="2">
         <v>13</v>
       </c>
@@ -85570,6 +85920,9 @@
       <c r="D4353" s="2">
         <v>1</v>
       </c>
+      <c r="G4353" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4353" s="2">
         <v>17</v>
       </c>
@@ -85587,6 +85940,9 @@
       <c r="D4354" s="2">
         <v>1</v>
       </c>
+      <c r="G4354" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4354" s="2">
         <v>2</v>
       </c>
@@ -85910,6 +86266,9 @@
       <c r="D4373" s="2">
         <v>2</v>
       </c>
+      <c r="G4373" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4373" s="2">
         <v>10</v>
       </c>
@@ -85927,6 +86286,9 @@
       <c r="D4374" s="2">
         <v>2</v>
       </c>
+      <c r="G4374" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4374" s="2">
         <v>10</v>
       </c>
@@ -85973,6 +86335,9 @@
       <c r="D4376" s="2">
         <v>2</v>
       </c>
+      <c r="G4376" s="2" t="s">
+        <v>765</v>
+      </c>
       <c r="K4376" s="2">
         <v>1</v>
       </c>
@@ -86312,6 +86677,9 @@
       <c r="D4391" s="2">
         <v>2</v>
       </c>
+      <c r="G4391" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4391" s="2">
         <v>10</v>
       </c>
@@ -86329,6 +86697,9 @@
       <c r="D4392" s="2">
         <v>2</v>
       </c>
+      <c r="G4392" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4392" s="2">
         <v>11</v>
       </c>
@@ -86346,6 +86717,9 @@
       <c r="D4393" s="2">
         <v>2</v>
       </c>
+      <c r="G4393" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4393" s="2">
         <v>17</v>
       </c>
@@ -86464,6 +86838,9 @@
       <c r="D4398" s="2">
         <v>10</v>
       </c>
+      <c r="G4398" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4398" s="2">
         <v>10</v>
       </c>
@@ -86925,6 +87302,9 @@
       <c r="E4420" s="1" t="s">
         <v>4910</v>
       </c>
+      <c r="G4420" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4420" s="2">
         <v>11</v>
       </c>
@@ -86945,6 +87325,9 @@
       <c r="E4421" s="1" t="s">
         <v>4911</v>
       </c>
+      <c r="G4421" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4421" s="2">
         <v>11</v>
       </c>
@@ -86965,6 +87348,9 @@
       <c r="E4422" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="G4422" s="2" t="s">
+        <v>699</v>
+      </c>
       <c r="K4422" s="2">
         <v>23</v>
       </c>
@@ -87771,6 +88157,9 @@
       <c r="C4456" s="2" t="s">
         <v>4675</v>
       </c>
+      <c r="G4456" s="2" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="4457" spans="1:11">
       <c r="A4457" s="2" t="s">
@@ -87910,6 +88299,9 @@
       <c r="D4464" s="2">
         <v>2</v>
       </c>
+      <c r="G4464" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="K4464" s="2">
         <v>1</v>
       </c>
@@ -87926,6 +88318,9 @@
       </c>
       <c r="D4465" s="2">
         <v>2</v>
+      </c>
+      <c r="G4465" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="K4465" s="2">
         <v>3</v>

</xml_diff>